<commit_message>
Added Swagger API Dcoumentation Completed Project
</commit_message>
<xml_diff>
--- a/appliedJobs.xlsx
+++ b/appliedJobs.xlsx
@@ -398,7 +398,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -473,9 +473,23 @@
         <v>44984.373703703706</v>
       </c>
     </row>
+    <row r="6">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>3</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6" s="1">
+        <v>44993.38872685185</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:D5"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:D6"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>